<commit_message>
sort out code table
</commit_message>
<xml_diff>
--- a/码表.xlsx
+++ b/码表.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HT1623" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="483">
   <si>
     <t xml:space="preserve">LCD RAM </t>
   </si>
@@ -1342,6 +1343,475 @@
     <t>20I</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>LCD RAM</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>D3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>D2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>COM0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>COM1</t>
+  </si>
+  <si>
+    <t>COM2</t>
+  </si>
+  <si>
+    <t>COM3</t>
+  </si>
+  <si>
+    <t>SEG10</t>
+  </si>
+  <si>
+    <t>SEG11</t>
+  </si>
+  <si>
+    <t>SEG12</t>
+  </si>
+  <si>
+    <t>SEG13</t>
+  </si>
+  <si>
+    <t>SEG14</t>
+  </si>
+  <si>
+    <t>SEG15</t>
+  </si>
+  <si>
+    <t>SEG16</t>
+  </si>
+  <si>
+    <t>SEG17</t>
+  </si>
+  <si>
+    <t>SEG18</t>
+  </si>
+  <si>
+    <t>SEG19</t>
+  </si>
+  <si>
+    <t>SEG20</t>
+  </si>
+  <si>
+    <t>SEG21</t>
+  </si>
+  <si>
+    <t>SEG22</t>
+  </si>
+  <si>
+    <t>SEG23</t>
+  </si>
+  <si>
+    <t>SEG24</t>
+  </si>
+  <si>
+    <t>SEG25</t>
+  </si>
+  <si>
+    <t>SEG26</t>
+  </si>
+  <si>
+    <t>SEG27</t>
+  </si>
+  <si>
+    <t>SEG28</t>
+  </si>
+  <si>
+    <t>SEG29</t>
+  </si>
+  <si>
+    <t>SEG30</t>
+  </si>
+  <si>
+    <t>SEG31</t>
+  </si>
+  <si>
+    <t>SEG32</t>
+  </si>
+  <si>
+    <t>SEG33</t>
+  </si>
+  <si>
+    <t>SEG34</t>
+  </si>
+  <si>
+    <t>SEG35</t>
+  </si>
+  <si>
+    <t>SEG36</t>
+  </si>
+  <si>
+    <t>SEG37</t>
+  </si>
+  <si>
+    <t>SEG38</t>
+  </si>
+  <si>
+    <t>SEG39</t>
+  </si>
+  <si>
+    <t>COM7</t>
+  </si>
+  <si>
+    <t>COM6</t>
+  </si>
+  <si>
+    <t>COM5</t>
+  </si>
+  <si>
+    <t>COM4</t>
+  </si>
+  <si>
+    <t>16F</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16I</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16J</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16K</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16L</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2K</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2I</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15F</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2L</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15L</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2F</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>6B</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>10B</t>
+  </si>
+  <si>
+    <t>15J</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15K</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15I</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>11I</t>
+  </si>
+  <si>
+    <t>11J</t>
+  </si>
+  <si>
+    <t>11K</t>
+  </si>
+  <si>
+    <t>20I</t>
+  </si>
+  <si>
+    <t>SEG00</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEG01</t>
+  </si>
+  <si>
+    <t>SEG02</t>
+  </si>
+  <si>
+    <t>SEG03</t>
+  </si>
+  <si>
+    <t>SEG04</t>
+  </si>
+  <si>
+    <t>SEG05</t>
+  </si>
+  <si>
+    <t>SEG06</t>
+  </si>
+  <si>
+    <t>SEG07</t>
+  </si>
+  <si>
+    <t>SEG08</t>
+  </si>
+  <si>
+    <t>SEG09</t>
+  </si>
+  <si>
+    <t>3K</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3J</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3I</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>6K</t>
+  </si>
+  <si>
+    <t>7K</t>
+  </si>
+  <si>
+    <t>14F</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>11F</t>
+  </si>
+  <si>
+    <t>11E</t>
+  </si>
+  <si>
+    <t>11C</t>
+  </si>
+  <si>
+    <t>3L</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>6L</t>
+  </si>
+  <si>
+    <t>7L</t>
+  </si>
+  <si>
+    <t>11G</t>
+  </si>
+  <si>
+    <t>11D</t>
+  </si>
+  <si>
+    <t>11A</t>
+  </si>
+  <si>
+    <t>3A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14L</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>11H</t>
+  </si>
+  <si>
+    <t>11M</t>
+  </si>
+  <si>
+    <t>11L</t>
+  </si>
+  <si>
+    <t>2J</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1350,7 +1820,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="&quot;0X&quot;@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="54">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1502,6 +1972,239 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF663300"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF663300"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF33CC"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF33CC"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF33CC33"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF33CC33"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF99CC00"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF99CC00"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0033CC"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0033CC"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC0066"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC0066"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF993366"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF993366"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6600FF"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6600FF"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6600CC"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6600CC"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FFFF"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1544,7 +2247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1608,6 +2311,129 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1615,6 +2441,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF0033CC"/>
+      <color rgb="FF6600CC"/>
+      <color rgb="FF993366"/>
+      <color rgb="FFCC0066"/>
+      <color rgb="FF003366"/>
+      <color rgb="FF33CC33"/>
+      <color rgb="FF6600FF"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FF99CC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1891,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42:J42"/>
+    <sheetView topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3433,4 +4273,1570 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:M44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="6.625" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>391</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>390</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>394</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>393</v>
+      </c>
+      <c r="F6" s="25">
+        <f>F5+2</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="25">
+        <f>K5+2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>401</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>399</v>
+      </c>
+      <c r="F7" s="25">
+        <f t="shared" ref="F7:F44" si="0">F6+2</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="25">
+        <f t="shared" ref="K7:K44" si="1">K6+2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="28" t="s">
+        <v>442</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>398</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>397</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>405</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>404</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="28" t="s">
+        <v>444</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>412</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>410</v>
+      </c>
+      <c r="F10" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>408</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>418</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>417</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>416</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>414</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="25">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>433</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>432</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>434</v>
+      </c>
+      <c r="F12" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>421</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="25">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>456</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>455</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>454</v>
+      </c>
+      <c r="F13" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>451</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>450</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>449</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>464</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>463</v>
+      </c>
+      <c r="F14" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>462</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>461</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>460</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="25">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>476</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>475</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>474</v>
+      </c>
+      <c r="F15" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>473</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>472</v>
+      </c>
+      <c r="I15" s="35" t="s">
+        <v>471</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="25">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="K16" s="25">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="25">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>264</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="F19" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="25">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>265</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="K20" s="25">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="25">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="25">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="25">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="25">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="28" t="s">
+        <v>364</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>301</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" s="25">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="25">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>261</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="F24" s="25">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="36" t="s">
+        <v>424</v>
+      </c>
+      <c r="K24" s="25">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="C25" s="59" t="s">
+        <v>459</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>458</v>
+      </c>
+      <c r="E25" s="59" t="s">
+        <v>457</v>
+      </c>
+      <c r="F25" s="25">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>452</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="25">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="C26" s="59" t="s">
+        <v>470</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>469</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>468</v>
+      </c>
+      <c r="F26" s="25">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>466</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="25">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>481</v>
+      </c>
+      <c r="D27" s="59" t="s">
+        <v>480</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>479</v>
+      </c>
+      <c r="F27" s="25">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27" s="38" t="s">
+        <v>477</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" s="25">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="C28" s="59" t="s">
+        <v>437</v>
+      </c>
+      <c r="D28" s="59" t="s">
+        <v>436</v>
+      </c>
+      <c r="E28" s="59" t="s">
+        <v>435</v>
+      </c>
+      <c r="F28" s="25">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" s="38" t="s">
+        <v>426</v>
+      </c>
+      <c r="J28" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="K28" s="25">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>307</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>281</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="E29" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29" s="25">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>453</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="25">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>282</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="E30" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="25">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="J30" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="25">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>283</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="E31" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="25">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="40" t="s">
+        <v>478</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="K31" s="25">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="D32" s="51" t="s">
+        <v>239</v>
+      </c>
+      <c r="E32" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="F32" s="25">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="I32" s="40" t="s">
+        <v>428</v>
+      </c>
+      <c r="J32" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="K32" s="25">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="B33" s="53" t="s">
+        <v>308</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>277</v>
+      </c>
+      <c r="D33" s="54" t="s">
+        <v>256</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>194</v>
+      </c>
+      <c r="F33" s="25">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="25">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" s="25">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="G34" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="25">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="25">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="I35" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="K35" s="25">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>280</v>
+      </c>
+      <c r="D36" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="F36" s="25">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="41" t="s">
+        <v>429</v>
+      </c>
+      <c r="K36" s="25">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="B37" s="60" t="s">
+        <v>311</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="D37" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="E37" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="F37" s="25">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="G37" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="H37" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="K37" s="25">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="C38" s="62" t="s">
+        <v>274</v>
+      </c>
+      <c r="D38" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="E38" s="62" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" s="25">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="G38" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="I38" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="K38" s="25">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="D39" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="E39" s="61" t="s">
+        <v>211</v>
+      </c>
+      <c r="F39" s="25">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="H39" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="K39" s="25">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="D40" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="F40" s="25">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="I40" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="J40" s="43" t="s">
+        <v>430</v>
+      </c>
+      <c r="K40" s="25">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="B41" s="63" t="s">
+        <v>314</v>
+      </c>
+      <c r="C41" s="63" t="s">
+        <v>269</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>254</v>
+      </c>
+      <c r="E41" s="63" t="s">
+        <v>192</v>
+      </c>
+      <c r="F41" s="25">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="G41" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="H41" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" s="25">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="C42" s="64" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" s="64" t="s">
+        <v>245</v>
+      </c>
+      <c r="E42" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="F42" s="25">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G42" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="H42" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="I42" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" s="25">
+        <f>K41+2</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="C43" s="63" t="s">
+        <v>271</v>
+      </c>
+      <c r="D43" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="F43" s="25">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="G43" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="H43" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="I43" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="J43" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="K43" s="25">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C44" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="D44" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="E44" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="F44" s="25">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="G44" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="H44" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="I44" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="J44" s="45" t="s">
+        <v>431</v>
+      </c>
+      <c r="K44" s="25">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add number change corresponding function
</commit_message>
<xml_diff>
--- a/码表.xlsx
+++ b/码表.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="501">
   <si>
     <t xml:space="preserve">LCD RAM </t>
   </si>
@@ -1810,6 +1810,74 @@
   </si>
   <si>
     <t>2J</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Digital_IJK</t>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Digital_HML</t>
+  </si>
+  <si>
+    <t>Digital_GDA</t>
+  </si>
+  <si>
+    <t>Digital_FECB</t>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -2206,7 +2274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2219,8 +2287,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2243,11 +2329,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2306,133 +2429,181 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2443,6 +2614,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF6600FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF0033CC"/>
       <color rgb="FF6600CC"/>
@@ -2450,7 +2622,6 @@
       <color rgb="FFCC0066"/>
       <color rgb="FF003366"/>
       <color rgb="FF33CC33"/>
-      <color rgb="FF6600FF"/>
       <color rgb="FFFF0000"/>
       <color rgb="FF99CC00"/>
     </mruColors>
@@ -2776,17 +2947,17 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="21" t="s">
@@ -3515,18 +3686,18 @@
       <c r="O24" s="9"/>
     </row>
     <row r="25" spans="1:15" ht="51" customHeight="1">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="64" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -3564,17 +3735,17 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="3"/>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="21" t="s">
@@ -4249,18 +4420,18 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="46.5" customHeight="1">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="64" t="s">
         <v>337</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4277,1564 +4448,2161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:M44"/>
+  <dimension ref="A3:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="6.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="6.625" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.25" style="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9" style="24"/>
+    <col min="3" max="5" width="6.625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="6.625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.25" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="24" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="1:29">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>389</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="26" t="s">
         <v>352</v>
       </c>
-      <c r="K3" s="28"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28" t="s">
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="26" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="28" t="s">
+      <c r="M4" s="23"/>
+      <c r="N4" s="65" t="s">
+        <v>483</v>
+      </c>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="68" t="s">
+        <v>487</v>
+      </c>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="71" t="s">
+        <v>488</v>
+      </c>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="74" t="s">
+        <v>489</v>
+      </c>
+      <c r="AA4" s="75"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="76"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="26" t="s">
         <v>439</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="46" t="s">
         <v>392</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="46" t="s">
         <v>391</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="46" t="s">
         <v>390</v>
       </c>
-      <c r="F5" s="25">
-        <v>1</v>
-      </c>
-      <c r="G5" s="29" t="s">
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="28" t="s">
+      <c r="M5" s="26" t="s">
+        <v>500</v>
+      </c>
+      <c r="N5" s="77" t="s">
+        <v>496</v>
+      </c>
+      <c r="O5" s="77" t="s">
+        <v>497</v>
+      </c>
+      <c r="P5" s="77" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q5" s="77" t="s">
+        <v>499</v>
+      </c>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78" t="s">
+        <v>493</v>
+      </c>
+      <c r="T5" s="78" t="s">
+        <v>494</v>
+      </c>
+      <c r="U5" s="78" t="s">
+        <v>495</v>
+      </c>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79" t="s">
+        <v>490</v>
+      </c>
+      <c r="X5" s="79" t="s">
+        <v>491</v>
+      </c>
+      <c r="Y5" s="79" t="s">
+        <v>492</v>
+      </c>
+      <c r="Z5" s="80"/>
+      <c r="AA5" s="80" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB5" s="80" t="s">
+        <v>485</v>
+      </c>
+      <c r="AC5" s="80" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="45" t="s">
         <v>395</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="46" t="s">
         <v>394</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="46" t="s">
         <v>393</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="23">
         <f>F5+2</f>
         <v>3</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="23">
         <f>K5+2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="28" t="s">
+      <c r="M6" s="47">
+        <v>1</v>
+      </c>
+      <c r="N6" s="77">
+        <v>1</v>
+      </c>
+      <c r="O6" s="77">
+        <v>1</v>
+      </c>
+      <c r="P6" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="77">
+        <v>1</v>
+      </c>
+      <c r="R6" s="78">
+        <v>0</v>
+      </c>
+      <c r="S6" s="78">
+        <v>0</v>
+      </c>
+      <c r="T6" s="78">
+        <v>1</v>
+      </c>
+      <c r="U6" s="78">
+        <v>0</v>
+      </c>
+      <c r="V6" s="79">
+        <v>0</v>
+      </c>
+      <c r="W6" s="79">
+        <v>0</v>
+      </c>
+      <c r="X6" s="79">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="79">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="80">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>401</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="46" t="s">
         <v>400</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <f t="shared" ref="F7:F44" si="0">F6+2</f>
         <v>5</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="23">
         <f t="shared" ref="K7:K44" si="1">K6+2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="28" t="s">
+      <c r="M7" s="47">
+        <v>2</v>
+      </c>
+      <c r="N7" s="77">
+        <v>1</v>
+      </c>
+      <c r="O7" s="77">
+        <v>0</v>
+      </c>
+      <c r="P7" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="77">
+        <v>1</v>
+      </c>
+      <c r="R7" s="78">
+        <v>0</v>
+      </c>
+      <c r="S7" s="78">
+        <v>1</v>
+      </c>
+      <c r="T7" s="78">
+        <v>1</v>
+      </c>
+      <c r="U7" s="78">
+        <v>1</v>
+      </c>
+      <c r="V7" s="79">
+        <v>0</v>
+      </c>
+      <c r="W7" s="79">
+        <v>1</v>
+      </c>
+      <c r="X7" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="80">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="46" t="s">
         <v>398</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="46" t="s">
         <v>396</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="23">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="28" t="s">
+      <c r="M8" s="47">
+        <v>3</v>
+      </c>
+      <c r="N8" s="77">
+        <v>1</v>
+      </c>
+      <c r="O8" s="77">
+        <v>1</v>
+      </c>
+      <c r="P8" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="77">
+        <v>1</v>
+      </c>
+      <c r="R8" s="78">
+        <v>0</v>
+      </c>
+      <c r="S8" s="78">
+        <v>1</v>
+      </c>
+      <c r="T8" s="78">
+        <v>1</v>
+      </c>
+      <c r="U8" s="78">
+        <v>1</v>
+      </c>
+      <c r="V8" s="79">
+        <v>0</v>
+      </c>
+      <c r="W8" s="79">
+        <v>1</v>
+      </c>
+      <c r="X8" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="47" t="s">
         <v>287</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>406</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="47" t="s">
         <v>405</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="47" t="s">
         <v>404</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="23">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="29" t="s">
         <v>403</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="30" t="s">
         <v>482</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="30" t="s">
         <v>402</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="23">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="28" t="s">
+      <c r="M9" s="47">
+        <v>4</v>
+      </c>
+      <c r="N9" s="77">
+        <v>1</v>
+      </c>
+      <c r="O9" s="77">
+        <v>1</v>
+      </c>
+      <c r="P9" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="77">
+        <v>1</v>
+      </c>
+      <c r="R9" s="78">
+        <v>0</v>
+      </c>
+      <c r="S9" s="78">
+        <v>0</v>
+      </c>
+      <c r="T9" s="78">
+        <v>1</v>
+      </c>
+      <c r="U9" s="78">
+        <v>0</v>
+      </c>
+      <c r="V9" s="79">
+        <v>0</v>
+      </c>
+      <c r="W9" s="79">
+        <v>0</v>
+      </c>
+      <c r="X9" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="26" t="s">
         <v>444</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="47" t="s">
         <v>412</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="47" t="s">
         <v>411</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="47" t="s">
         <v>410</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="23">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="30" t="s">
         <v>409</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="30" t="s">
         <v>408</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="30" t="s">
         <v>407</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="23">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="28" t="s">
+      <c r="M10" s="47">
+        <v>5</v>
+      </c>
+      <c r="N10" s="77">
+        <v>1</v>
+      </c>
+      <c r="O10" s="77">
+        <v>1</v>
+      </c>
+      <c r="P10" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="77">
+        <v>1</v>
+      </c>
+      <c r="R10" s="78">
+        <v>0</v>
+      </c>
+      <c r="S10" s="78">
+        <v>1</v>
+      </c>
+      <c r="T10" s="78">
+        <v>1</v>
+      </c>
+      <c r="U10" s="78">
+        <v>1</v>
+      </c>
+      <c r="V10" s="79">
+        <v>0</v>
+      </c>
+      <c r="W10" s="79">
+        <v>1</v>
+      </c>
+      <c r="X10" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="47" t="s">
         <v>418</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="47" t="s">
         <v>417</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="47" t="s">
         <v>416</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="23">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="30" t="s">
         <v>415</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="30" t="s">
         <v>414</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="23">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="28" t="s">
+      <c r="M11" s="47">
+        <v>6</v>
+      </c>
+      <c r="N11" s="77">
+        <v>1</v>
+      </c>
+      <c r="O11" s="77">
+        <v>1</v>
+      </c>
+      <c r="P11" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="77">
+        <v>1</v>
+      </c>
+      <c r="R11" s="78">
+        <v>0</v>
+      </c>
+      <c r="S11" s="78">
+        <v>1</v>
+      </c>
+      <c r="T11" s="78">
+        <v>1</v>
+      </c>
+      <c r="U11" s="78">
+        <v>1</v>
+      </c>
+      <c r="V11" s="79">
+        <v>0</v>
+      </c>
+      <c r="W11" s="79">
+        <v>1</v>
+      </c>
+      <c r="X11" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="80">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="26" t="s">
         <v>446</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="47" t="s">
         <v>432</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="47" t="s">
         <v>434</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="23">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="30" t="s">
         <v>421</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="30" t="s">
         <v>420</v>
       </c>
-      <c r="I12" s="32" t="s">
+      <c r="I12" s="30" t="s">
         <v>419</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="23">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="28" t="s">
+      <c r="M12" s="47">
+        <v>7</v>
+      </c>
+      <c r="N12" s="77">
+        <v>1</v>
+      </c>
+      <c r="O12" s="77">
+        <v>1</v>
+      </c>
+      <c r="P12" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="77">
+        <v>1</v>
+      </c>
+      <c r="R12" s="78">
+        <v>0</v>
+      </c>
+      <c r="S12" s="78">
+        <v>0</v>
+      </c>
+      <c r="T12" s="78">
+        <v>1</v>
+      </c>
+      <c r="U12" s="78">
+        <v>1</v>
+      </c>
+      <c r="V12" s="79">
+        <v>0</v>
+      </c>
+      <c r="W12" s="79">
+        <v>0</v>
+      </c>
+      <c r="X12" s="79">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="80">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13" s="26" t="s">
         <v>447</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="49" t="s">
         <v>456</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="49" t="s">
         <v>455</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="49" t="s">
         <v>454</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="23">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="33" t="s">
         <v>451</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="33" t="s">
         <v>450</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="I13" s="33" t="s">
         <v>449</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="23">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="28" t="s">
+      <c r="M13" s="47">
+        <v>8</v>
+      </c>
+      <c r="N13" s="77">
+        <v>1</v>
+      </c>
+      <c r="O13" s="77">
+        <v>1</v>
+      </c>
+      <c r="P13" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="77">
+        <v>1</v>
+      </c>
+      <c r="R13" s="78">
+        <v>0</v>
+      </c>
+      <c r="S13" s="78">
+        <v>1</v>
+      </c>
+      <c r="T13" s="78">
+        <v>1</v>
+      </c>
+      <c r="U13" s="78">
+        <v>1</v>
+      </c>
+      <c r="V13" s="79">
+        <v>0</v>
+      </c>
+      <c r="W13" s="79">
+        <v>1</v>
+      </c>
+      <c r="X13" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="80">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" s="26" t="s">
         <v>448</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="50" t="s">
         <v>465</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="50" t="s">
         <v>464</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="50" t="s">
         <v>463</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="23">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="33" t="s">
         <v>462</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="33" t="s">
         <v>461</v>
       </c>
-      <c r="I14" s="35" t="s">
+      <c r="I14" s="33" t="s">
         <v>460</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="23">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="28" t="s">
+      <c r="M14" s="47">
+        <v>9</v>
+      </c>
+      <c r="N14" s="77">
+        <v>1</v>
+      </c>
+      <c r="O14" s="77">
+        <v>1</v>
+      </c>
+      <c r="P14" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="77">
+        <v>1</v>
+      </c>
+      <c r="R14" s="78">
+        <v>0</v>
+      </c>
+      <c r="S14" s="78">
+        <v>1</v>
+      </c>
+      <c r="T14" s="78">
+        <v>1</v>
+      </c>
+      <c r="U14" s="78">
+        <v>1</v>
+      </c>
+      <c r="V14" s="79">
+        <v>0</v>
+      </c>
+      <c r="W14" s="79">
+        <v>1</v>
+      </c>
+      <c r="X14" s="79">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="26" t="s">
         <v>356</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="49" t="s">
         <v>476</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="49" t="s">
         <v>475</v>
       </c>
-      <c r="E15" s="51" t="s">
+      <c r="E15" s="49" t="s">
         <v>474</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="33" t="s">
         <v>473</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="33" t="s">
         <v>472</v>
       </c>
-      <c r="I15" s="35" t="s">
+      <c r="I15" s="33" t="s">
         <v>471</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="23">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="28" t="s">
+      <c r="M15" s="47">
+        <v>0</v>
+      </c>
+      <c r="N15" s="77">
+        <v>1</v>
+      </c>
+      <c r="O15" s="77">
+        <v>1</v>
+      </c>
+      <c r="P15" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="77">
+        <v>1</v>
+      </c>
+      <c r="R15" s="78">
+        <v>0</v>
+      </c>
+      <c r="S15" s="78">
+        <v>1</v>
+      </c>
+      <c r="T15" s="78">
+        <v>1</v>
+      </c>
+      <c r="U15" s="78">
+        <v>1</v>
+      </c>
+      <c r="V15" s="79">
+        <v>0</v>
+      </c>
+      <c r="W15" s="79">
+        <v>1</v>
+      </c>
+      <c r="X15" s="79">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="79">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="80">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="80">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="80">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="23">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="I16" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="25" t="s">
         <v>422</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="23">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="51" t="s">
         <v>295</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="52" t="s">
         <v>262</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="52" t="s">
         <v>250</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="23">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H17" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="23">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D18" s="53" t="s">
         <v>241</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="23">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="23">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="57" t="s">
         <v>297</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="52" t="s">
         <v>264</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="52" t="s">
         <v>231</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="23">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="52" t="s">
         <v>223</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="23">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="33" t="s">
+      <c r="J20" s="31" t="s">
         <v>423</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="23">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="54" t="s">
         <v>299</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="55" t="s">
         <v>258</v>
       </c>
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="55" t="s">
         <v>249</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="55" t="s">
         <v>187</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="23">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="23">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="26" t="s">
         <v>363</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="56" t="s">
         <v>259</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="E22" s="58" t="s">
+      <c r="E22" s="56" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="23">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="23">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>364</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="55" t="s">
         <v>260</v>
       </c>
-      <c r="D23" s="57" t="s">
+      <c r="D23" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="23">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="I23" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="23">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="55" t="s">
         <v>261</v>
       </c>
-      <c r="D24" s="57" t="s">
+      <c r="D24" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="23">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="I24" s="29" t="s">
+      <c r="I24" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="36" t="s">
+      <c r="J24" s="34" t="s">
         <v>424</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="23">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="26" t="s">
         <v>366</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="57" t="s">
         <v>459</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="57" t="s">
         <v>458</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="57" t="s">
         <v>457</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="23">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="H25" s="38" t="s">
+      <c r="H25" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="I25" s="38" t="s">
+      <c r="I25" s="36" t="s">
         <v>452</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="23">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="26" t="s">
         <v>367</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="57" t="s">
         <v>470</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="57" t="s">
         <v>469</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="57" t="s">
         <v>468</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="23">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="H26" s="38" t="s">
+      <c r="H26" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="38" t="s">
+      <c r="I26" s="36" t="s">
         <v>466</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="23">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="C27" s="59" t="s">
+      <c r="C27" s="57" t="s">
         <v>481</v>
       </c>
-      <c r="D27" s="59" t="s">
+      <c r="D27" s="57" t="s">
         <v>480</v>
       </c>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="57" t="s">
         <v>479</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="23">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="G27" s="38" t="s">
+      <c r="G27" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="H27" s="38" t="s">
+      <c r="H27" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="I27" s="38" t="s">
+      <c r="I27" s="36" t="s">
         <v>477</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="J27" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="23">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="26" t="s">
         <v>369</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="57" t="s">
         <v>437</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="57" t="s">
         <v>436</v>
       </c>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="23">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="38" t="s">
+      <c r="H28" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="I28" s="38" t="s">
+      <c r="I28" s="36" t="s">
         <v>426</v>
       </c>
-      <c r="J28" s="37" t="s">
+      <c r="J28" s="35" t="s">
         <v>425</v>
       </c>
-      <c r="K28" s="25">
+      <c r="K28" s="23">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="26" t="s">
         <v>370</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="D29" s="51" t="s">
+      <c r="D29" s="49" t="s">
         <v>257</v>
       </c>
-      <c r="E29" s="51" t="s">
+      <c r="E29" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="23">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="H29" s="40" t="s">
+      <c r="H29" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="38" t="s">
         <v>453</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="23">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="26" t="s">
         <v>371</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="50" t="s">
         <v>282</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="23">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="H30" s="40" t="s">
+      <c r="H30" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I30" s="38" t="s">
         <v>467</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="J30" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="25">
+      <c r="K30" s="23">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="26" t="s">
         <v>372</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="49" t="s">
         <v>283</v>
       </c>
-      <c r="D31" s="51" t="s">
+      <c r="D31" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="49" t="s">
         <v>213</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="23">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="H31" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="I31" s="38" t="s">
         <v>478</v>
       </c>
-      <c r="J31" s="25" t="s">
+      <c r="J31" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="K31" s="25">
+      <c r="K31" s="23">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="49" t="s">
         <v>284</v>
       </c>
-      <c r="D32" s="51" t="s">
+      <c r="D32" s="49" t="s">
         <v>239</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="49" t="s">
         <v>438</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="23">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="H32" s="40" t="s">
+      <c r="H32" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="I32" s="40" t="s">
+      <c r="I32" s="38" t="s">
         <v>428</v>
       </c>
-      <c r="J32" s="39" t="s">
+      <c r="J32" s="37" t="s">
         <v>427</v>
       </c>
-      <c r="K32" s="25">
+      <c r="K32" s="23">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="26" t="s">
         <v>374</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="54" t="s">
+      <c r="D33" s="52" t="s">
         <v>256</v>
       </c>
-      <c r="E33" s="54" t="s">
+      <c r="E33" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="23">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K33" s="25">
+      <c r="K33" s="23">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="53" t="s">
         <v>278</v>
       </c>
-      <c r="D34" s="55" t="s">
+      <c r="D34" s="53" t="s">
         <v>247</v>
       </c>
-      <c r="E34" s="55" t="s">
+      <c r="E34" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="23">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="G34" s="42" t="s">
+      <c r="G34" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="H34" s="42" t="s">
+      <c r="H34" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="I34" s="42" t="s">
+      <c r="I34" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K34" s="25">
+      <c r="K34" s="23">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="26" t="s">
         <v>376</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="52" t="s">
         <v>279</v>
       </c>
-      <c r="D35" s="54" t="s">
+      <c r="D35" s="52" t="s">
         <v>237</v>
       </c>
-      <c r="E35" s="54" t="s">
+      <c r="E35" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="23">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="G35" s="42" t="s">
+      <c r="G35" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="H35" s="42" t="s">
+      <c r="H35" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="I35" s="42" t="s">
+      <c r="I35" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="J35" s="25" t="s">
+      <c r="J35" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="K35" s="25">
+      <c r="K35" s="23">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C36" s="52" t="s">
         <v>280</v>
       </c>
-      <c r="D36" s="54" t="s">
+      <c r="D36" s="52" t="s">
         <v>229</v>
       </c>
-      <c r="E36" s="54" t="s">
+      <c r="E36" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="23">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="G36" s="42" t="s">
+      <c r="G36" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="H36" s="42" t="s">
+      <c r="H36" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="I36" s="42" t="s">
+      <c r="I36" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="J36" s="41" t="s">
+      <c r="J36" s="39" t="s">
         <v>429</v>
       </c>
-      <c r="K36" s="25">
+      <c r="K36" s="23">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="61" t="s">
+      <c r="C37" s="59" t="s">
         <v>273</v>
       </c>
-      <c r="D37" s="61" t="s">
+      <c r="D37" s="59" t="s">
         <v>255</v>
       </c>
-      <c r="E37" s="61" t="s">
+      <c r="E37" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="23">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="G37" s="43" t="s">
+      <c r="G37" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="H37" s="44" t="s">
+      <c r="H37" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="J37" s="25" t="s">
+      <c r="J37" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="K37" s="25">
+      <c r="K37" s="23">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="C38" s="62" t="s">
+      <c r="C38" s="60" t="s">
         <v>274</v>
       </c>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="60" t="s">
         <v>246</v>
       </c>
-      <c r="E38" s="62" t="s">
+      <c r="E38" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="F38" s="25">
+      <c r="F38" s="23">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="G38" s="44" t="s">
+      <c r="G38" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="H38" s="44" t="s">
+      <c r="H38" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="I38" s="44" t="s">
+      <c r="I38" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="J38" s="25" t="s">
+      <c r="J38" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="K38" s="25">
+      <c r="K38" s="23">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="26" t="s">
         <v>380</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="59" t="s">
         <v>275</v>
       </c>
-      <c r="D39" s="61" t="s">
+      <c r="D39" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="E39" s="61" t="s">
+      <c r="E39" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="F39" s="25">
+      <c r="F39" s="23">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="G39" s="44" t="s">
+      <c r="G39" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="H39" s="44" t="s">
+      <c r="H39" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="I39" s="44" t="s">
+      <c r="I39" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="J39" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="K39" s="25">
+      <c r="K39" s="23">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="59" t="s">
         <v>276</v>
       </c>
-      <c r="D40" s="61" t="s">
+      <c r="D40" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="E40" s="61" t="s">
+      <c r="E40" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="23">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="G40" s="44" t="s">
+      <c r="G40" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="H40" s="44" t="s">
+      <c r="H40" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="I40" s="44" t="s">
+      <c r="I40" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="J40" s="43" t="s">
+      <c r="J40" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="K40" s="25">
+      <c r="K40" s="23">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="61" t="s">
         <v>314</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="61" t="s">
         <v>269</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="E41" s="63" t="s">
+      <c r="E41" s="61" t="s">
         <v>192</v>
       </c>
-      <c r="F41" s="25">
+      <c r="F41" s="23">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="G41" s="45" t="s">
+      <c r="G41" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="H41" s="46" t="s">
+      <c r="H41" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="I41" s="46" t="s">
+      <c r="I41" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="J41" s="26" t="s">
+      <c r="J41" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K41" s="25">
+      <c r="K41" s="23">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="26" t="s">
         <v>383</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="C42" s="64" t="s">
+      <c r="C42" s="62" t="s">
         <v>270</v>
       </c>
-      <c r="D42" s="64" t="s">
+      <c r="D42" s="62" t="s">
         <v>245</v>
       </c>
-      <c r="E42" s="64" t="s">
+      <c r="E42" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="F42" s="25">
+      <c r="F42" s="23">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G42" s="46" t="s">
+      <c r="G42" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="H42" s="46" t="s">
+      <c r="H42" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="I42" s="46" t="s">
+      <c r="I42" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="J42" s="26" t="s">
+      <c r="J42" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="K42" s="25">
+      <c r="K42" s="23">
         <f>K41+2</f>
         <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="61" t="s">
         <v>271</v>
       </c>
-      <c r="D43" s="63" t="s">
+      <c r="D43" s="61" t="s">
         <v>235</v>
       </c>
-      <c r="E43" s="63" t="s">
+      <c r="E43" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="23">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="G43" s="46" t="s">
+      <c r="G43" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="I43" s="46" t="s">
+      <c r="I43" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="J43" s="25" t="s">
+      <c r="J43" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="K43" s="25">
+      <c r="K43" s="23">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="26" t="s">
         <v>385</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="C44" s="63" t="s">
+      <c r="C44" s="61" t="s">
         <v>272</v>
       </c>
-      <c r="D44" s="63" t="s">
+      <c r="D44" s="61" t="s">
         <v>227</v>
       </c>
-      <c r="E44" s="63" t="s">
+      <c r="E44" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="F44" s="25">
+      <c r="F44" s="23">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="G44" s="46" t="s">
+      <c r="G44" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="H44" s="46" t="s">
+      <c r="H44" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="I44" s="46" t="s">
+      <c r="I44" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="J44" s="45" t="s">
+      <c r="J44" s="43" t="s">
         <v>431</v>
       </c>
-      <c r="K44" s="25">
+      <c r="K44" s="23">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="Z4:AC4"/>
+  </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>